<commit_message>
met nose, zonder dome
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -117,9 +117,6 @@
     <t>Calculations</t>
   </si>
   <si>
-    <t>Weight of the tailplanes using Class II weight estimation methods</t>
-  </si>
-  <si>
     <t>Areas for all lifting surfaces from 3D geometry models</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -669,20 +669,20 @@
     </row>
     <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -707,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
@@ -750,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -766,12 +766,12 @@
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -782,17 +782,17 @@
     </row>
     <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -819,13 +819,13 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C34" s="6" t="s">
         <v>27</v>
       </c>
@@ -835,71 +835,71 @@
         <v>25</v>
       </c>
       <c r="C36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
         <v>55</v>
-      </c>
-      <c r="D36" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C39" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
         <v>59</v>
-      </c>
-      <c r="D39" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C40" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" t="s">
         <v>34</v>
-      </c>
-      <c r="D43" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C44" s="4"/>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C45" s="4"/>
       <c r="D45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
@@ -908,28 +908,28 @@
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
       <c r="D47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C48" s="4"/>
       <c r="D48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C49" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C50" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C51" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
@@ -937,51 +937,51 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" t="s">
         <v>53</v>
-      </c>
-      <c r="D60" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>